<commit_message>
constructor metaclass acceleo operations has been added
</commit_message>
<xml_diff>
--- a/comparation-ccsl-vs-pmd.xlsx
+++ b/comparation-ccsl-vs-pmd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-repositories\Coding-Conventions-Specification-Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D810080-E31A-41A5-B8F9-6C805F3C218F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9211DA93-A93A-4574-BA9E-0DC8BF19BD98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>PMD Rule Id</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t xml:space="preserve">The result of OCL should select only nodes that originalCompilationUnit is not null </t>
+  </si>
+  <si>
+    <t>category/java/performance.xml/BigIntegerInstantiation</t>
+  </si>
+  <si>
+    <t>BooleanInstantiation</t>
+  </si>
+  <si>
+    <t>category/java/performance.xml/BooleanInstantiation</t>
+  </si>
+  <si>
+    <t>category/java/performance.xml/ByteInstantiation</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,6 +531,54 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>